<commit_message>
Add BioPAN test file
</commit_message>
<xml_diff>
--- a/test/test_output/test_equalize.xlsx
+++ b/test/test_output/test_equalize.xlsx
@@ -4,11 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Lv_B1_matched" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Lv_B1_unmatched" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Lv_B2_matched" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Lv_B2_unmatched" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="skipped" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -56,18 +56,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -439,7 +439,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID@Lv_B1</t>
+          <t>ID@Lv_B2</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -505,7 +505,11 @@
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cer(d18:0/26:0(3OH))</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Cer 44:0;2O</t>
@@ -513,7 +517,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Cer 18:0;2O/26:0</t>
+          <t>Cer 18:0;2O/26:0;(3OH)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -540,7 +544,11 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cer(t18:0/26:0)</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Cer 44:0;3O</t>
@@ -548,7 +556,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cer 18:0;3O/26:0</t>
+          <t>Cer 18:0;3O/26:0;(3OH)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -610,7 +618,11 @@
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Cer(d18:1/26:0(3OH))</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>Cer 44:1;2O</t>
@@ -618,7 +630,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Cer 18:1;2O/26:0</t>
+          <t>Cer 18:1;2O/26:0;(3OH)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -703,13 +715,13 @@
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>DG(O-16:0/18:1&lt;{9Z}&gt;)</t>
+          <t>DG(O-16:0/18:1)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>DG(O-16:0/18:1(9Z))</t>
+          <t>DG(O-16:0/18:1)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
@@ -1297,7 +1309,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>TG(16:0_18:2_20:4&lt;+16&gt;)</t>
+          <t>TG(16:0_18:2_20:4&lt;O&gt;)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1407,7 +1419,7 @@
       <c r="I30" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1417,7 +1429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1428,7 +1440,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID@Lv_B1</t>
+          <t>ID@Lv_B2</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -1453,15 +1465,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SOURCE_07</t>
+          <t>SOURCE_08</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>SOURCE_08</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>SOURCE_09</t>
         </is>
@@ -1483,174 +1490,164 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0)</t>
+          <t>Cer(59:0;O5)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Cer(t18:0/26:0)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Cer 59:0;5O</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0;O2&lt;+16&gt;)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>FA14:0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FA14:0</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Cer 18:0;2O/26:0;(3OH)</t>
-        </is>
-      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0;O3&lt;+16&gt;)</t>
+          <t>FA18:1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>oleic acid</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Cer 18:0;3O/26:0;(3OH)</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0&lt;+16&gt;)</t>
+          <t>FA20:4&lt;O&gt;</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Cer(d18:0/26:0(3OH))</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>HETE</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:1;O2&lt;+16&gt;)</t>
+          <t>LPE(O-16:1)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Cer 18:1;2O/26:0;(3OH)</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LPE P-16:0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:1&lt;+16&gt;)</t>
+          <t>LPE(O-18:1)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Cer(d18:1/26:0(3OH))</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LPE O-18:1</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Cer(59:0;O5)</t>
+          <t>PC(32:0)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Cer 59:0;5O</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>DPPC</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FA14:0</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>FA14:0</t>
-        </is>
-      </c>
+          <t>PC(34:0)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GPCho(17:0/17:0)</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FA18:1</t>
+          <t>PC(34:1)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>oleic acid</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>POPC</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>FA20:4&lt;+16&gt;</t>
+          <t>PC(34:2)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1658,53 +1655,50 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>HETE</t>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>PLPC</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>LPE(O-16:1)</t>
+          <t>PC(36:4)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>LPE P-16:0</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>PAPC</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>LPE(O-18:1)</t>
+          <t>PE(32:0)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LPE O-18:1</t>
-        </is>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>DPPE</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>PC(32:0)</t>
+          <t>PE(34:1)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1712,17 +1706,16 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>DPPC</t>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>POPE</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>PC(34:0)</t>
+          <t>PE(36:4)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1732,265 +1725,148 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>GPCho(17:0/17:0)</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
+          <t>PAPE</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>PC(34:1)</t>
+          <t>PE(37:5)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>GPEtn(15:0/22:5(4Z,7Z,10Z,13Z,16Z))</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>POPC</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>PC(34:2)</t>
+          <t>PE(40:6)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>GPEtn(20:3(5Z,8Z,11Z)/20:3(5Z,8Z,11Z))</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>PLPC</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>PC(36:4)</t>
+          <t>PE(O-16:1)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>PE(P-16:0)</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>PAPC</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>PE(32:0)</t>
+          <t>PE(O-18:1)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>PE(O-18:1)</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>DPPE</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>PE(34:1)</t>
+          <t>PE(O-38:5)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>PE(P-16:0/22:4(7Z,10Z,13Z,16Z))</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>POPE</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>PE(36:4)</t>
+          <t>PI(38:4)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>GPIns(18:0/20:4(5E,8E,11E,14E))</t>
+        </is>
+      </c>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>PAPE</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>PE(37:5)</t>
+          <t>PS(40:6)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>GPEtn(15:0/22:5(4Z,7Z,10Z,13Z,16Z))</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>GPSer(18:0/22:6(4Z,7Z,10Z,13Z,16Z,19Z))</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>PE(40:6)</t>
+          <t>SM(44:1;O2)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>SM(d18:1/26:0)</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>GPEtn(20:3(5Z,8Z,11Z)/20:3(5Z,8Z,11Z))</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>PE(O-16:1)</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>PE(P-16:0)</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>PE(O-18:1)</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>PE(O-18:1)</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>PE(O-38:5)</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>PE(P-16:0/22:4(7Z,10Z,13Z,16Z))</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>PI(38:4)</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>GPIns(18:0/20:4(5E,8E,11E,14E))</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>PS(40:6)</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>GPSer(18:0/22:6(4Z,7Z,10Z,13Z,16Z,19Z))</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>SM(44:1)</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>SM(d18:1/26:0)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2798,6 +2674,6 @@
       <c r="I27" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update SPB/SPBP for BioPAN
</commit_message>
<xml_diff>
--- a/test/test_output/test_equalize.xlsx
+++ b/test/test_output/test_equalize.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,221 +486,157 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0;O2)</t>
+          <t>DG(34:2)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cer(44:0;2)</t>
+          <t>DG(34:2)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cer(18:0;2/26:0&lt;OH{3}&gt;)</t>
+          <t>DG(16:0/18:2)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cer(18:0;2/26:0&lt;OH{3}&gt;)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>DG(16:0/18:2)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>DG(34:2)</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cer(d18:0/26:0(3OH))</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Cer 44:0;2O</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Cer 18:0;2O/26:0;(3OH)</t>
-        </is>
-      </c>
+          <t>DG(16:0/18:2(9Z,12Z)/0:0)[iso2]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0;O3)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Cer(44:0;3)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Cer(18:0;3/26:0&lt;OH{3}&gt;)</t>
-        </is>
-      </c>
+          <t>DG(O-34:1)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cer(18:0;3/26:0&lt;OH{3}&gt;)</t>
+          <t>DG(O-16:0/18:1)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cer(t18:0/26:0)</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Cer 44:0;3O</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Cer 18:0;3O/26:0;(3OH)</t>
-        </is>
-      </c>
+          <t>DG(O-16:0/18:1)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:0;O4)</t>
+          <t>DG(O-34:2)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cer(44:0;4)</t>
+          <t>DG(O-34:2)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Cer(18:0;3/26:0;1)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Cer(18:0;3/26:0;1)</t>
-        </is>
-      </c>
+          <t>DG(O-16:0/18:2)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Cer 44:0;4O</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Cer 18:0;3O/26:0;O</t>
-        </is>
-      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:1;O2)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cer(44:1;2)</t>
-        </is>
-      </c>
+          <t>DG(O-34:3)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cer(18:1;2/26:0&lt;OH{3}&gt;)</t>
+          <t>DG(P-16:0/18:2)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Cer(18:1;2/26:0&lt;OH{3}&gt;)</t>
+          <t>DG(P-16:0/18:2)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Cer(d18:1/26:0(3OH))</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Cer 44:1;2O</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Cer 18:1;2O/26:0;(3OH)</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Cer(44:1;O3)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cer(44:1;3)</t>
-        </is>
-      </c>
+          <t>FA16:0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Cer(18:1;2/26:0;1)</t>
+          <t>FA16:0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cer(18:1;2/26:0;1)</t>
+          <t>FA16:0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>palmitic acid</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cer 44:1;3O</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Cer 18:1;2O/26:0;O</t>
-        </is>
-      </c>
+          <t>FA 16:0</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>DG(34:2)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>DG(34:2)</t>
-        </is>
-      </c>
+          <t>FA18:2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DG(16:0/18:2)</t>
+          <t>FA18:2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DG(16:0/18:2)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>DG(34:2)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>DG(16:0/18:2(9Z,12Z)/0:0)[iso2]</t>
-        </is>
-      </c>
+          <t>FA18:2&lt;{9Z,12Z}&gt;</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -708,180 +644,224 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>DG(O-34:1)</t>
+          <t>FA22:6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>FA22:6</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>DG(O-16:0/18:1)</t>
+          <t>FA22:6&lt;{4Z,7Z,10Z,13Z,16Z,19Z}&gt;</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>DG(O-16:0/18:1)</t>
+          <t>Docosahexaenoic acid</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>DHA</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>DG(O-34:2)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>DG(O-34:2)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>DG(O-16:0/18:2)</t>
-        </is>
-      </c>
+          <t>LPE(16:0)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LPE 16:0 </t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>LPE 16:0/0:0</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>DG(O-34:3)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>DG(P-34:2)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>DG(P-16:0/18:2)</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>DG(P-16:0/18:2)</t>
-        </is>
-      </c>
+          <t>LPIP(16:0)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LPIP 16:0 </t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>LPIP 16:0/0:0</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FA16:0</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
+          <t>MG(16:0)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MG(16:0)</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FA16:0</t>
+          <t>MG(16:0)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>FA16:0</t>
+          <t>MG(16:0)</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>palmitic acid</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>FA 16:0</t>
-        </is>
-      </c>
+          <t>MG(16:0)</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>FA18:2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+          <t>PE(34:2)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PE(34:2)</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>FA18:2</t>
+          <t>PE(16:0_18:2)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FA18:2&lt;{9Z,12Z}&gt;</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+          <t>PE(16:0/18:2)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>PE(34:2)</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>PE(16:0/18:2(9Z,12Z))</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>PE 34:2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>PE 16:0_18:2</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>FA22:6</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+          <t>PE(O-34:2)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PE(O-34:2)</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>FA22:6</t>
+          <t>PE(O-16:0_18:2)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FA22:6&lt;{4Z,7Z,10Z,13Z,16Z,19Z}&gt;</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>PE(O-16:0/18:2)</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>PE(O-34:2)</t>
+        </is>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Docosahexaenoic acid</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>DHA</t>
-        </is>
-      </c>
+          <t>PE(O-16:0/18:2(9Z,12Z))</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>PE O-34:2</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>PE O-16:0_18:2</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>LPE(16:0)</t>
+          <t>PE(O-34:3)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PE(P-16:0_18:2)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PE(P-16:0/18:2)</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">LPE 16:0 </t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>PE(P-16:0/18:2(9Z,12Z))</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>LPE 16:0/0:0</t>
+          <t>PE P-16:0_18:2</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -889,534 +869,284 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>LPIP(16:0)</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+          <t>PE(P-34:2)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PE(P-34:2)</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>PE(P-34:2)</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve">LPIP 16:0 </t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>LPIP 16:0/0:0</t>
-        </is>
-      </c>
+          <t>PE P-34:2</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>MG(16:0)</t>
+          <t>PIP(34:1)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MG(16:0)</t>
+          <t>PIP(34:1)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>MG(16:0)</t>
+          <t>PIP(16:0_18:1)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MG(16:0)</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>MG(16:0)</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
+          <t>PIP(16:0/18:1)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>PIP(34:1)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>PIP 34:1</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>PE(34:2)</t>
+          <t>PIP2(34:2)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PE(34:2)</t>
+          <t>PIP2(34:2)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PE(16:0_18:2)</t>
+          <t>PIP2(16:0_18:2)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>PE(16:0/18:2)</t>
+          <t>PIP2(16:0/18:2)</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>PE(34:2)</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>PE(16:0/18:2(9Z,12Z))</t>
-        </is>
-      </c>
+          <t>PIP2(34:2)</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
-          <t>PE 34:2</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>PE 16:0_18:2</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>PLPE</t>
-        </is>
-      </c>
+          <t>PIP2 34:2</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>PE(34:2;O2)</t>
+          <t>PIP3(34:2)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PE(34:2;2)</t>
+          <t>PIP3(34:2)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PE(18:2;2_16:0)</t>
+          <t>PIP3(16:0_18:2)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>PE(18:2;2/16:0)</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>PIP3(16:0/18:2)</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>PIP3(34:2)</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>PIP3 34:2</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>PE(O-34:2)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>PE(O-34:2)</t>
-        </is>
-      </c>
+          <t>SPB18:0</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>PE(O-16:0_18:2)</t>
+          <t>SPB18:0;2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PE(O-16:0/18:2)</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>PE(O-34:2)</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>PE(O-16:0/18:2(9Z,12Z))</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>PE O-34:2</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>PE O-16:0_18:2</t>
-        </is>
-      </c>
+          <t>SPB18:0;2</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>PE(O-34:3)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>PE(P-34:2)</t>
-        </is>
-      </c>
+          <t>SPB18:1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PE(P-16:0_18:2)</t>
+          <t>SPB18:1;2</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PE(P-16:0/18:2)</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>PE(P-34:2)</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>PE(P-16:0/18:2(9Z,12Z))</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>PE P-34:2</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>PE P-16:0_18:2</t>
-        </is>
-      </c>
+          <t>SPB18:1;2</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>PIP(34:1)</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>PIP(34:1)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>PIP(16:0_18:1)</t>
-        </is>
-      </c>
+          <t>TG(16:0_18:2_20:4&lt;+O&gt;)</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PIP(16:0/18:1)</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>PIP(34:1)</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>PIP 34:1</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>PIP 16:0_18:1</t>
-        </is>
-      </c>
+          <t>TG(16:0/18:2/20:4&lt;OH&gt;)</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>TG(16:0/18:2/HETE)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>PIP2(34:2)</t>
+          <t>TG(52:2)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PIP2(34:2)</t>
+          <t>TG(52:2)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PIP2(16:0_18:2)</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>PIP2(16:0/18:2)</t>
-        </is>
-      </c>
+          <t>TG(16:0/18:2/18:0)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>PIP2(34:2)</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>PIP2 34:2</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>PIP2 16:0_18:2</t>
-        </is>
-      </c>
+          <t>TG(52:2)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>TG(16:0/18:0/18:2(9Z,12Z))[iso6]</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>PIP3(34:2)</t>
+          <t>TG(O-52:2)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PIP3(34:2)</t>
+          <t>TG(O-52:2)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PIP3(16:0_18:2)</t>
+          <t>TG(O-16:0/18:2/18:0)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>PIP3(16:0/18:2)</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>PIP3(34:2)</t>
-        </is>
-      </c>
+          <t>TG(O-16:0/18:2/18:0)</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>PIP3 34:2</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>PIP3 16:0_18:2</t>
-        </is>
-      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>SM(34:1;O2)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>SM(34:1;2)</t>
-        </is>
-      </c>
+          <t>TG(O-52:3)</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SM(18:1;2/16:0)</t>
+          <t>TG(P-16:0/18:2/18:0)</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>SM(18:1;2/16:0)</t>
+          <t>TG(P-16:0/18:2/18:0)</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>SM 34:1;2O</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>SM 18:1;2O/16:0</t>
-        </is>
-      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>SPB18:0;O2</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>SPB18:0;2</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>SPB18:0;2</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>SPB 18:0;2O</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>SPB 18:0;2O</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>SPB18:1;O2</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>SPB18:1;2</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>SPB18:1;2</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>TG(16:0_18:2_20:4&lt;O&gt;)</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>TG(16:0/18:2/20:4&lt;OH&gt;)</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>TG(16:0/18:2/HETE)</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>TG(52:2)</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>TG(52:2)</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>TG(16:0/18:2/18:0)</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>TG(16:0/18:2&lt;{9Z,12Z}&gt;/18:0)</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>TG(52:2)</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>TG(16:0/18:0/18:2(9Z,12Z))[iso6]</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>TG(O-52:2)</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>TG(O-52:2)</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>TG(O-16:0/18:2/18:0)</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>TG(O-16:0/18:2/18:0)</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>TG(O-52:3)</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>TG(P-52:2)</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>TG(P-16:0/18:2/18:0)</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>TG(P-16:0/18:2/18:0)</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1429,7 +1159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1465,10 +1195,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>SOURCE_07</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>SOURCE_08</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>SOURCE_09</t>
         </is>
@@ -1490,181 +1225,192 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Cer(59:0;O5)</t>
+          <t>Cer(44:0;2O)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Cer 59:0;5O</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cer(d18:0/26:0)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>FA14:0</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>FA14:0</t>
-        </is>
-      </c>
+          <t>Cer(44:0;2O&lt;+3O&gt;)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cer(d18:0/26:0(3OH))</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>FA18:1</t>
+          <t>Cer(44:0;3O)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>oleic acid</t>
+          <t>Cer(t18:0/26:0)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>FA20:4&lt;O&gt;</t>
+          <t>Cer(44:1;2O&lt;+3O&gt;)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Cer(d18:1/26:0(3OH))</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>HETE</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>LPE(O-16:1)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>DG(P-34:2)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>DG(P-34:2)</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LPE P-16:0</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>LPE(O-18:1)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr"/>
+          <t>FA14:0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>FA14:0</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>LPE O-18:1</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>PC(32:0)</t>
+          <t>FA18:1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>oleic acid</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>DPPC</t>
-        </is>
-      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>PC(34:0)</t>
+          <t>FA20:4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>GPCho(17:0/17:0)</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>HETE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>PC(34:1)</t>
+          <t>LPE(O-18:1)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LPE O-18:1</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>POPC</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>PC(34:2)</t>
+          <t>LPE(P-16:0)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>LPE P-16:0</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>PLPC</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>PC(36:4)</t>
+          <t>PC(32:0)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1672,9 +1418,10 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>PAPC</t>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>DPPC</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1436,8 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>DPPE</t>
         </is>
@@ -1698,24 +1446,25 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>PE(34:1)</t>
+          <t>PE(O-18:1)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>PE(O-18:1)</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>POPE</t>
-        </is>
-      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>PE(36:4)</t>
+          <t>PE(O-38:5)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1725,31 +1474,33 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
-          <t>PAPE</t>
-        </is>
-      </c>
+          <t>PE(P-16:0/22:4(7Z,10Z,13Z,16Z))</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>PE(37:5)</t>
+          <t>PE(P-16:0)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PE(P-16:0)</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>GPEtn(15:0/22:5(4Z,7Z,10Z,13Z,16Z))</t>
-        </is>
-      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>PE(40:6)</t>
+          <t>PIP(16:0)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1758,112 +1509,83 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>GPEtn(20:3(5Z,8Z,11Z)/20:3(5Z,8Z,11Z))</t>
+          <t>PIP 16:0_18:1</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>PE(O-16:1)</t>
+          <t>PIP2(16:0)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>PE(P-16:0)</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>PIP2 16:0_18:2</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>PE(O-18:1)</t>
+          <t>PIP3(16:0)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>PE(O-18:1)</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>PIP3 16:0_18:2</t>
+        </is>
+      </c>
       <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>PE(O-38:5)</t>
+          <t>SM(44:1;2O)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>SM(d18:1/26:0)</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>PE(P-16:0/22:4(7Z,10Z,13Z,16Z))</t>
-        </is>
-      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>PI(38:4)</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
+          <t>TG(P-52:2)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TG(P-52:2)</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>GPIns(18:0/20:4(5E,8E,11E,14E))</t>
-        </is>
-      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>PS(40:6)</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>GPSer(18:0/22:6(4Z,7Z,10Z,13Z,16Z,19Z))</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>SM(44:1;O2)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>SM(d18:1/26:0)</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1876,7 +1598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1934,15 +1656,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>PE(34:2;2)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>PE(18:2;2_16:0)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PE(18:2;2/16:0)</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1955,33 +1681,41 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:0;3O</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;2O/26:0;(2OH)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GPCho(17:0/17:0)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>PLPC</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+          <t>Cer(44:0;2)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0)</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>nan</t>
@@ -1994,33 +1728,41 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:0;3O</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;2O/26:0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GPEtn(18:0/22:6(4Z,7Z,10Z,13Z,16Z,19Z))</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>POPC</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+          <t>Cer(44:0;3)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0;1)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0;1)</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2033,33 +1775,41 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:0;3O</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;2O/26:0;(3OH)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GPEtn(15:0/22:5(4Z,7Z,10Z,13Z,16Z))</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>PAPC</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+          <t>Cer(44:0;3)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0&lt;OH{2}&gt;)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0&lt;OH{2}&gt;)</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2072,29 +1822,41 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:0;4O</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;2O/26:0;O</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GPEtn(20:3(5Z,8Z,11Z)/20:3(5Z,8Z,11Z))</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>PLPE</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Cer(44:0;3)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0&lt;OH{3}&gt;)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cer(18:0;2/26:0&lt;OH{3}&gt;)</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2107,29 +1869,41 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:0;4O</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;3O/26:0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GPIns(18:0/20:4(5E,8E,11E,14E))</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>POPE</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cer(44:1;2)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0)</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2142,29 +1916,41 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:0;4O</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;3O/26:0;(3OH)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>GPSer(18:0/22:6(4Z,7Z,10Z,13Z,16Z,19Z))</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>PAPE</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cer(44:1;3)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0;1)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0;1)</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2177,12 +1963,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 44:1;3O</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:0;3O/26:0;O</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -2197,9 +1983,21 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Cer(44:1;3)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0&lt;OH{2}&gt;)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0&lt;OH{2}&gt;)</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2210,10 +2008,14 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Cer 44:1;3O</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:1;2O/26:0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -2228,9 +2030,21 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cer(44:1;3)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0&lt;OH{3}&gt;)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Cer(18:1;2/26:0&lt;OH{3}&gt;)</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2241,10 +2055,14 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Cer 44:1;3O</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:1;2O/26:0;(3OH)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -2259,9 +2077,21 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cer(44:0;3)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0)</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2272,10 +2102,14 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Cer 59:0;5O</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cer 18:1;2O/26:0;O</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -2290,9 +2124,21 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cer(44:0;4)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0;1)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0;1)</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2303,10 +2149,14 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Cer 44:0;2O</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SM 18:1;2O/16:0</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -2321,9 +2171,21 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Cer(44:0;4)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0&lt;OH{2R}&gt;)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0&lt;OH{2R}&gt;)</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2334,10 +2196,14 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Cer 44:0;3O</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SPB 18:0;2O</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -2352,9 +2218,21 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Cer(44:0;4)</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0&lt;OH{3}&gt;)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Cer(18:0;3/26:0&lt;OH{3}&gt;)</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2365,7 +2243,11 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Cer 44:1;2O</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2383,9 +2265,21 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SM(34:1;2)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SM(18:1;2/16:0)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SM(18:1;2/16:0)</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2396,8 +2290,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>SM 34:1;2O</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H15" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2410,9 +2312,21 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>TG(16:0/18:2&lt;{9Z,12Z}&gt;/18:0)</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2423,8 +2337,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>SPB 18:0;2O</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H16" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2437,7 +2359,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
@@ -2450,8 +2376,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H17" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2464,7 +2398,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
@@ -2477,8 +2415,16 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H18" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2491,7 +2437,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
@@ -2500,8 +2450,16 @@
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H19" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2523,8 +2481,16 @@
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H20" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2546,8 +2512,16 @@
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2569,8 +2543,16 @@
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H22" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2592,8 +2574,16 @@
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H23" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2616,7 +2606,11 @@
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
           <t>nan</t>
@@ -2635,13 +2629,21 @@
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H25" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -2650,13 +2652,21 @@
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
           <t>nan</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -2671,7 +2681,113 @@
           <t>nan</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>